<commit_message>
basic benchmarked models attempted
</commit_message>
<xml_diff>
--- a/sourceData/dietSubsets/1009_A_B_y.xlsx
+++ b/sourceData/dietSubsets/1009_A_B_y.xlsx
@@ -1,15 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenlianfu/Documents/GitHub/IBS_FructanSensitivity/sourceData/dietSubsets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA50A42-9DA5-604C-9C3E-2E6DE912DD73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="16180" yWindow="4580" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -22,8 +40,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +104,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -132,7 +158,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -164,9 +190,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -198,6 +242,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -373,339 +435,341 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>0</v>
       </c>

</xml_diff>